<commit_message>
Created scripts for crdc prog-study fields
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/Section-B.xlsx
+++ b/InputFiles/CRDC/Section-B.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F856C18-2E78-493A-AF02-F48486C00EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25882FB0-6232-4662-880A-D9ABFD9831C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1849FEBB-C412-4D13-84D0-137F35324848}"/>
+    <workbookView xWindow="4272" yWindow="1620" windowWidth="17280" windowHeight="8976" activeTab="2" xr2:uid="{1849FEBB-C412-4D13-84D0-137F35324848}"/>
   </bookViews>
   <sheets>
     <sheet name="program-study" sheetId="1" r:id="rId1"/>
-    <sheet name="publication-info" sheetId="3" r:id="rId2"/>
-    <sheet name="planned-publication-info" sheetId="4" r:id="rId3"/>
-    <sheet name="repository-info" sheetId="5" r:id="rId4"/>
-    <sheet name="agency-info" sheetId="6" r:id="rId5"/>
+    <sheet name="funding-agency-dbGaP" sheetId="3" r:id="rId2"/>
+    <sheet name="publication-repository" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>program</t>
   </si>
@@ -99,12 +97,6 @@
     <t>Division of Cancer Control and Population Sciences</t>
   </si>
   <si>
-    <t>Katalon-Test</t>
-  </si>
-  <si>
-    <t>K-T</t>
-  </si>
-  <si>
     <t>NCI's Childhood Cancer Data Initiative (CCDI) is building a community centered around childhood cancer care and research data.</t>
   </si>
   <si>
@@ -130,13 +122,154 @@
   </si>
   <si>
     <t>prog-abbreviation</t>
+  </si>
+  <si>
+    <t>Department of Defense (DoD)</t>
+  </si>
+  <si>
+    <t>National Cancer Institute (NCI)</t>
+  </si>
+  <si>
+    <t>Veterans Affairs (VA)</t>
+  </si>
+  <si>
+    <t>grant-number</t>
+  </si>
+  <si>
+    <t>nci-prog-officer</t>
+  </si>
+  <si>
+    <t>James Alberto</t>
+  </si>
+  <si>
+    <t>Rocky Max</t>
+  </si>
+  <si>
+    <t>Sebren Natt</t>
+  </si>
+  <si>
+    <t>nci-genomic-prog-admin</t>
+  </si>
+  <si>
+    <t>Daniel Mathew</t>
+  </si>
+  <si>
+    <t>John Ricks</t>
+  </si>
+  <si>
+    <t>Walter Steve</t>
+  </si>
+  <si>
+    <t>stdy-registerd-dbGap</t>
+  </si>
+  <si>
+    <t>dbgap-phs-num</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>phs001980</t>
+  </si>
+  <si>
+    <t>phs001974</t>
+  </si>
+  <si>
+    <t>publication-title</t>
+  </si>
+  <si>
+    <t>Test-Title-Publication Two</t>
+  </si>
+  <si>
+    <t>Test-Title-Publication Three</t>
+  </si>
+  <si>
+    <t>Test-Title-Publication One</t>
+  </si>
+  <si>
+    <t>pubmed-id</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>pland-publictn-title</t>
+  </si>
+  <si>
+    <t>Test-Title-PlanedPublication One</t>
+  </si>
+  <si>
+    <t>Test-Title-PlanedPublication Two</t>
+  </si>
+  <si>
+    <t>Test-Title-PlanedPublication Three</t>
+  </si>
+  <si>
+    <t>exptd-pubtn-date</t>
+  </si>
+  <si>
+    <t>Use system date for this</t>
+  </si>
+  <si>
+    <t>repository-name</t>
+  </si>
+  <si>
+    <t>study-id</t>
+  </si>
+  <si>
+    <t>data-types-submtd</t>
+  </si>
+  <si>
+    <t>data-commons-repo-2</t>
+  </si>
+  <si>
+    <t>data-commons-repo-3</t>
+  </si>
+  <si>
+    <t>data-commons-repo-1</t>
+  </si>
+  <si>
+    <t>Clinical Trial</t>
+  </si>
+  <si>
+    <t>Genomics</t>
+  </si>
+  <si>
+    <t>Imaging</t>
+  </si>
+  <si>
+    <t>Immunology</t>
+  </si>
+  <si>
+    <t>Proteomics</t>
+  </si>
+  <si>
+    <t>Epidemiologic or Cohort</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Katalon-Test-</t>
+  </si>
+  <si>
+    <t>KT-</t>
+  </si>
+  <si>
+    <t>other-data-types</t>
+  </si>
+  <si>
+    <t>TestOtherDataType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,19 +284,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -172,9 +374,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,43 +700,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF7C09E-E14D-4823-832B-9C902D6A7F0A}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="121" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="33.77734375" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -534,13 +748,13 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -554,7 +768,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -568,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -582,7 +796,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -596,7 +810,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,13 +818,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -621,58 +835,260 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9F0A03-590F-4531-BA87-E357A61B34FB}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>34543543345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>34543566464</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>23454545646</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0294DDC2-A1B7-42D4-8BE2-759203EBA80B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7701C2-D09C-4563-903C-4136618228C4}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27538E1-4B37-4BD1-AED2-F31CD15184B2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECB94E6-BEAE-4389-A72F-BC214DF517EE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>340598943</v>
+      </c>
+      <c r="C2">
+        <v>456456</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2">
+        <v>234324</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>345345345</v>
+      </c>
+      <c r="C3">
+        <v>545645</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="3">
+        <v>55110</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3">
+        <v>235325</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>323894354</v>
+      </c>
+      <c r="C4">
+        <v>345334</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="3">
+        <v>55111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4">
+        <v>235232</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>